<commit_message>
Correct emission factors in local_grid_parameters.xlsx
</commit_message>
<xml_diff>
--- a/pvcompare/data/static_inputs/local_grid_parameters.xlsx
+++ b/pvcompare/data/static_inputs/local_grid_parameters.xlsx
@@ -286,10 +286,10 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.07"/>
@@ -346,7 +346,7 @@
         <v>0.05</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>250</v>
+        <v>0.25</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>0.15</v>
@@ -363,7 +363,7 @@
         <v>0.0497101083032491</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>207</v>
+        <v>0.207</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>0.099</v>
@@ -380,7 +380,7 @@
         <v>0.0397509025270758</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>425</v>
+        <v>0.425</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>0.21</v>
@@ -397,7 +397,7 @@
         <v>0.0574256317689531</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>445</v>
+        <v>0.445</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>0.162</v>
@@ -414,7 +414,7 @@
         <v>0.0751938628158845</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>189</v>
+        <v>0.189</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>0.37</v>
@@ -434,7 +434,7 @@
         <v>0.1197</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>338</v>
+        <v>0.338</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>0.174</v>
@@ -451,7 +451,7 @@
         <v>0.0442429602888087</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>900</v>
+        <v>0.9</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>0.319</v>
@@ -468,7 +468,7 @@
         <v>0.0670880866425993</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>353</v>
+        <v>0.353</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>0.12</v>
@@ -488,7 +488,7 @@
         <v>0.115</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>662</v>
+        <v>0.662</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>0.197</v>
@@ -505,7 +505,7 @@
         <v>0.0719527075812275</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>207</v>
+        <v>0.207</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>0.184</v>
@@ -525,7 +525,7 @@
         <v>0.144</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>54</v>
+        <v>0.054</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>0.172</v>
@@ -542,7 +542,7 @@
         <v>0.0389761732851986</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>135</v>
+        <v>0.135</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>0.285</v>
@@ -559,7 +559,7 @@
         <v>0.0730274368231047</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>248</v>
+        <v>0.248</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>0.182</v>
@@ -573,7 +573,7 @@
         <v>0.2133</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>664</v>
+        <v>0.664</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>0.138</v>
@@ -590,7 +590,7 @@
         <v>0.0315707581227437</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>138</v>
+        <v>0.138</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>0.41</v>
@@ -610,7 +610,7 @@
         <v>0.1419</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>65</v>
+        <v>0.065</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>0.255</v>
@@ -630,7 +630,7 @@
         <v>0.1312</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>69</v>
+        <v>0.069</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>0.07</v>
@@ -650,7 +650,7 @@
         <v>0.09</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>251</v>
+        <v>0.251</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>0.126</v>
@@ -667,7 +667,7 @@
         <v>0.155</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>356</v>
+        <v>0.356</v>
       </c>
       <c r="F21" s="1" t="n">
         <v>0.085</v>
@@ -684,7 +684,7 @@
         <v>0.099784476534296</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>441</v>
+        <v>0.441</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>0.088</v>
@@ -704,7 +704,7 @@
         <v>0.0791</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>102</v>
+        <v>0.102</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>0.336</v>
@@ -721,7 +721,7 @@
         <v>0.0426223826714801</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>789</v>
+        <v>0.789</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>0.122</v>
@@ -738,7 +738,7 @@
         <v>0.0787418772563177</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>310</v>
+        <v>0.31</v>
       </c>
       <c r="F25" s="1" t="n">
         <v>0.306</v>
@@ -755,7 +755,7 @@
         <v>0.0324837545126354</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>293</v>
+        <v>0.293</v>
       </c>
       <c r="F26" s="1" t="n">
         <v>0.243</v>
@@ -772,7 +772,7 @@
         <v>0.0587559566787004</v>
       </c>
       <c r="E27" s="1" t="n">
-        <v>248</v>
+        <v>0.248</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>0.22</v>
@@ -789,7 +789,7 @@
         <v>0.0458628158844765</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>137</v>
+        <v>0.137</v>
       </c>
       <c r="F28" s="1" t="n">
         <v>0.169</v>
@@ -803,7 +803,7 @@
         <v>0.174</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>111</v>
+        <v>0.111</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>0.431</v>
@@ -820,7 +820,7 @@
         <v>0.0982729241877256</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>13</v>
+        <v>0.013</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>0.564</v>
@@ -840,7 +840,7 @@
         <v>0.115</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>250</v>
+        <v>0.25</v>
       </c>
       <c r="F31" s="1" t="n">
         <v>0.123</v>
@@ -882,7 +882,7 @@
         <v>0.1355</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>19</v>
+        <v>0.019</v>
       </c>
       <c r="F34" s="1" t="n">
         <v>0.746</v>

</xml_diff>